<commit_message>
Final. If run script please delete CPV from aggregrated
</commit_message>
<xml_diff>
--- a/output/CPV.xlsx
+++ b/output/CPV.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,52 +451,27 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>1. Mean air temperature</t>
+          <t>4. Agriculture land area (% of land area)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>4. Agriculture land area (% of land area)_x</t>
+          <t>5. Average precipitation (mm per year)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>4. Agriculture land area (% of land area)_y</t>
+          <t>7. Fertilizer consumption (kilograms per hectare of arable land)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>5. Average precipitation (mm)</t>
+          <t>13. Population</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>7. Fertilizer consumption (kilograms per hectare of arable land)_x</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>7. Fertilizer consumption (kilograms per hectare of arable land)_y</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>13. Population_x</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>13. Population_y</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>17. Employment in agriculture (% of total employment) (modeled ILO estimate)_x</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>17. Employment in agriculture (% of total employment) (modeled ILO estimate)_y</t>
+          <t>17. Employment in agriculture (% of total employment) (modeled ILO estimate)</t>
         </is>
       </c>
     </row>
@@ -507,42 +482,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1997</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>49.68</t>
-        </is>
+        <v>2015</v>
+      </c>
+      <c r="C2" t="n">
+        <v>101.41</v>
       </c>
       <c r="D2" t="n">
-        <v>23.09</v>
+        <v>19.60297767</v>
       </c>
       <c r="E2" t="n">
-        <v>17.86600496</v>
+        <v>228</v>
       </c>
       <c r="F2" t="n">
-        <v>17.86600496</v>
+        <v>3.0346</v>
       </c>
       <c r="G2" t="n">
-        <v>125.37</v>
+        <v>552166</v>
       </c>
       <c r="H2" t="n">
-        <v>2.318181818</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2.318181818</v>
-      </c>
-      <c r="J2" t="n">
-        <v>430654</v>
-      </c>
-      <c r="K2" t="n">
-        <v>430654</v>
-      </c>
-      <c r="L2" t="n">
-        <v>32.6455739613823</v>
-      </c>
-      <c r="M2" t="n">
-        <v>32.6455739613823</v>
+        <v>15.76179647527</v>
       </c>
     </row>
     <row r="3">
@@ -552,42 +510,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1998</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>52.39</t>
-        </is>
+        <v>2016</v>
+      </c>
+      <c r="C3" t="n">
+        <v>98.06</v>
       </c>
       <c r="D3" t="n">
-        <v>23.14</v>
+        <v>19.60297767</v>
       </c>
       <c r="E3" t="n">
-        <v>17.86600496</v>
+        <v>228</v>
       </c>
       <c r="F3" t="n">
-        <v>17.86600496</v>
+        <v>3.0816</v>
       </c>
       <c r="G3" t="n">
-        <v>145.98</v>
+        <v>558394</v>
       </c>
       <c r="H3" t="n">
-        <v>2.590909091</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2.590909091</v>
-      </c>
-      <c r="J3" t="n">
-        <v>440214</v>
-      </c>
-      <c r="K3" t="n">
-        <v>440214</v>
-      </c>
-      <c r="L3" t="n">
-        <v>31.6164603587673</v>
-      </c>
-      <c r="M3" t="n">
-        <v>31.6164603587673</v>
+        <v>14.7118964486198</v>
       </c>
     </row>
     <row r="4">
@@ -597,42 +538,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1999</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>75.22</t>
-        </is>
+        <v>2017</v>
+      </c>
+      <c r="C4" t="n">
+        <v>91.26000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>23.15</v>
+        <v>19.60297767</v>
       </c>
       <c r="E4" t="n">
-        <v>17.86600496</v>
+        <v>228</v>
       </c>
       <c r="F4" t="n">
-        <v>17.86600496</v>
+        <v>3.9134</v>
       </c>
       <c r="G4" t="n">
-        <v>148.15</v>
+        <v>564954</v>
       </c>
       <c r="H4" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="I4" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="J4" t="n">
-        <v>449627</v>
-      </c>
-      <c r="K4" t="n">
-        <v>449627</v>
-      </c>
-      <c r="L4" t="n">
-        <v>30.5989232839838</v>
-      </c>
-      <c r="M4" t="n">
-        <v>30.5989232839838</v>
+        <v>13.6167403600925</v>
       </c>
     </row>
     <row r="5">
@@ -642,42 +566,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>99.6</t>
-        </is>
+        <v>2018</v>
+      </c>
+      <c r="C5" t="n">
+        <v>72.04000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>23.27</v>
+        <v>19.60297767</v>
       </c>
       <c r="E5" t="n">
-        <v>17.86600496</v>
+        <v>228</v>
       </c>
       <c r="F5" t="n">
-        <v>17.86600496</v>
+        <v>4.07</v>
       </c>
       <c r="G5" t="n">
-        <v>118.98</v>
+        <v>571202</v>
       </c>
       <c r="H5" t="n">
-        <v>2.931818182</v>
-      </c>
-      <c r="I5" t="n">
-        <v>2.931818182</v>
-      </c>
-      <c r="J5" t="n">
-        <v>458251</v>
-      </c>
-      <c r="K5" t="n">
-        <v>458251</v>
-      </c>
-      <c r="L5" t="n">
-        <v>29.2854404606048</v>
-      </c>
-      <c r="M5" t="n">
-        <v>29.2854404606048</v>
+        <v>11.8382835657588</v>
       </c>
     </row>
     <row r="6">
@@ -687,42 +594,81 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>97.26</t>
-        </is>
+        <v>2019</v>
+      </c>
+      <c r="C6" t="n">
+        <v>70.18000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>23.42</v>
+        <v>19.60297767</v>
       </c>
       <c r="E6" t="n">
-        <v>18.36228288</v>
+        <v>228</v>
       </c>
       <c r="F6" t="n">
-        <v>18.36228288</v>
+        <v>4.0876</v>
       </c>
       <c r="G6" t="n">
-        <v>144.98</v>
+        <v>577030</v>
       </c>
       <c r="H6" t="n">
-        <v>5.282608696</v>
-      </c>
-      <c r="I6" t="n">
-        <v>5.282608696</v>
-      </c>
-      <c r="J6" t="n">
-        <v>465958</v>
-      </c>
-      <c r="K6" t="n">
-        <v>465958</v>
-      </c>
-      <c r="L6" t="n">
-        <v>28.5888984158666</v>
-      </c>
-      <c r="M6" t="n">
-        <v>28.5888984158666</v>
+        <v>10.6044463385184</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CPV</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C7" t="n">
+        <v>69.34</v>
+      </c>
+      <c r="D7" t="n">
+        <v>19.60297767</v>
+      </c>
+      <c r="E7" t="n">
+        <v>228</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5.6728</v>
+      </c>
+      <c r="G7" t="n">
+        <v>582640</v>
+      </c>
+      <c r="H7" t="n">
+        <v>10.743090600802</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CPV</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C8" t="n">
+        <v>70.52</v>
+      </c>
+      <c r="D8" t="n">
+        <v>19.60297767</v>
+      </c>
+      <c r="E8" t="n">
+        <v>228</v>
+      </c>
+      <c r="F8" t="n">
+        <v>5.373</v>
+      </c>
+      <c r="G8" t="n">
+        <v>587925</v>
+      </c>
+      <c r="H8" t="n">
+        <v>10.5378314239351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>